<commit_message>
Buggy decomposition of antwerpen (works but with some help)
</commit_message>
<xml_diff>
--- a/test_data/antwerpen.xlsx
+++ b/test_data/antwerpen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\GitHub\Adaptive-Sonar-Route-Planning\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E09F9DB-66EA-4F70-BD81-8F7657482702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835142D3-EA0B-4EF6-8105-3414B6825FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{66C3736A-0E62-4634-AFEE-C53C0DACC39D}"/>
   </bookViews>
@@ -32,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="1">
   <si>
     <t>#</t>
   </si>
@@ -897,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0858634E-E16C-4A18-A6CA-53242E1B96DD}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,7 +930,7 @@
     <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -918,11 +940,24 @@
       <c r="C1" s="1">
         <v>216516.70170000001</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" cm="1">
+        <f t="array" ref="D1:D50">B1:B50-G1</f>
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" cm="1">
+        <f t="array" ref="E1:E50">C1:C50-H1</f>
+        <v>98.455699999991339</v>
+      </c>
+      <c r="G1" s="1">
+        <f>MIN(B1:B50)</f>
+        <v>146917.83350000001</v>
+      </c>
+      <c r="H1" s="1">
+        <f>MIN(C1:C50)</f>
+        <v>216418.24600000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -932,11 +967,14 @@
       <c r="C2" s="1">
         <v>216418.24600000001</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="1">
+        <v>182.43260000000009</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -946,11 +984,14 @@
       <c r="C3" s="1">
         <v>216904.73300000001</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" s="1">
+        <v>457.52939999999944</v>
+      </c>
+      <c r="E3">
+        <v>486.48699999999371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -960,11 +1001,14 @@
       <c r="C4" s="1">
         <v>216780.21549999999</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>674.71109999998589</v>
+      </c>
+      <c r="E4">
+        <v>361.96949999997742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -974,11 +1018,14 @@
       <c r="C5" s="1">
         <v>216539.86780000001</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>833.97759999998379</v>
+      </c>
+      <c r="E5">
+        <v>121.62179999999353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -988,11 +1035,14 @@
       <c r="C6" s="1">
         <v>216719.40460000001</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>949.80789999998524</v>
+      </c>
+      <c r="E6">
+        <v>301.1585999999952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1002,11 +1052,14 @@
       <c r="C7" s="1">
         <v>216980.0226</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>784.7497999999905</v>
+      </c>
+      <c r="E7">
+        <v>561.77659999998286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1016,11 +1069,14 @@
       <c r="C8" s="1">
         <v>217252.2237</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>764.47949999998673</v>
+      </c>
+      <c r="E8">
+        <v>833.97769999998854</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1030,11 +1086,17 @@
       <c r="C9" s="1">
         <v>217336.20060000001</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>631.27469999997993</v>
+      </c>
+      <c r="E9">
+        <v>917.9545999999973</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1046,11 +1108,14 @@
         <f>217365.1581</f>
         <v>217365.1581</v>
       </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>631.27469999997993</v>
+      </c>
+      <c r="E10">
+        <v>946.91209999998682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1060,11 +1125,17 @@
       <c r="C11" s="1">
         <v>217677.89970000001</v>
       </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>970.07819999998901</v>
+      </c>
+      <c r="E11">
+        <v>1259.6536999999953</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1074,11 +1145,17 @@
       <c r="C12" s="1">
         <v>217683.69130000001</v>
       </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>1022.2017999999807</v>
+      </c>
+      <c r="E12">
+        <v>1265.4452999999921</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1088,11 +1165,17 @@
       <c r="C13" s="1">
         <v>218230.98910000001</v>
       </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>1471.0438999999897</v>
+      </c>
+      <c r="E13">
+        <v>1812.7430999999924</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1102,11 +1185,17 @@
       <c r="C14" s="1">
         <v>218228.09330000001</v>
       </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>1618.7274000000034</v>
+      </c>
+      <c r="E14">
+        <v>1809.847299999994</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1116,11 +1205,17 @@
       <c r="C15" s="1">
         <v>217411.4902</v>
       </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>2759.6551999999792</v>
+      </c>
+      <c r="E15">
+        <v>993.24419999998645</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1130,11 +1225,17 @@
       <c r="C16" s="1">
         <v>217394.11569999999</v>
       </c>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>3199.8099999999977</v>
+      </c>
+      <c r="E16">
+        <v>975.86969999998109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1144,11 +1245,17 @@
       <c r="C17" s="1">
         <v>217469.40530000001</v>
       </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>3246.1420999999973</v>
+      </c>
+      <c r="E17">
+        <v>1051.1592999999993</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1158,11 +1265,17 @@
       <c r="C18" s="1">
         <v>219012.8431</v>
       </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>1308.8815999999933</v>
+      </c>
+      <c r="E18">
+        <v>2594.5970999999845</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1172,11 +1285,17 @@
       <c r="C19" s="1">
         <v>218564.00099999999</v>
       </c>
-      <c r="E19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>883.20549999998184</v>
+      </c>
+      <c r="E19">
+        <v>2145.7549999999756</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1186,11 +1305,17 @@
       <c r="C20" s="1">
         <v>218549.52220000001</v>
       </c>
-      <c r="E20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>900.57999999998719</v>
+      </c>
+      <c r="E20">
+        <v>2131.276199999993</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1200,11 +1325,17 @@
       <c r="C21" s="1">
         <v>218468.44099999999</v>
       </c>
-      <c r="E21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>793.437099999981</v>
+      </c>
+      <c r="E21">
+        <v>2050.1949999999779</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1214,11 +1345,17 @@
       <c r="C22" s="1">
         <v>218488.7113</v>
       </c>
-      <c r="E22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>761.58369999998831</v>
+      </c>
+      <c r="E22">
+        <v>2070.4652999999817</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1228,11 +1365,17 @@
       <c r="C23" s="1">
         <v>218462.6495</v>
       </c>
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <v>729.73040000000037</v>
+      </c>
+      <c r="E23">
+        <v>2044.4034999999858</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1242,11 +1385,17 @@
       <c r="C24" s="1">
         <v>218413.42170000001</v>
       </c>
-      <c r="E24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <v>755.79219999999623</v>
+      </c>
+      <c r="E24">
+        <v>1995.1756999999925</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1256,11 +1405,17 @@
       <c r="C25" s="1">
         <v>218303.383</v>
       </c>
-      <c r="E25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>613.90020000000368</v>
+      </c>
+      <c r="E25">
+        <v>1885.1369999999879</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1270,11 +1425,17 @@
       <c r="C26" s="1">
         <v>218329.4448</v>
       </c>
-      <c r="E26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>567.56810000000405</v>
+      </c>
+      <c r="E26">
+        <v>1911.1987999999837</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1284,11 +1445,17 @@
       <c r="C27" s="1">
         <v>218306.2787</v>
       </c>
-      <c r="E27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>538.61059999998542</v>
+      </c>
+      <c r="E27">
+        <v>1888.0326999999816</v>
+      </c>
+      <c r="F27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1298,11 +1465,17 @@
       <c r="C28" s="1">
         <v>218288.90419999999</v>
       </c>
-      <c r="E28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>558.88079999998445</v>
+      </c>
+      <c r="E28">
+        <v>1870.6581999999762</v>
+      </c>
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1312,11 +1485,17 @@
       <c r="C29" s="1">
         <v>218222.30179999999</v>
       </c>
-      <c r="E29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>483.5911999999953</v>
+      </c>
+      <c r="E29">
+        <v>1804.0557999999728</v>
+      </c>
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1326,11 +1505,17 @@
       <c r="C30" s="1">
         <v>218036.97349999999</v>
       </c>
-      <c r="E30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>674.71109999998589</v>
+      </c>
+      <c r="E30">
+        <v>1618.727499999979</v>
+      </c>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1340,11 +1525,17 @@
       <c r="C31" s="1">
         <v>217938.5178</v>
       </c>
-      <c r="E31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>321.42889999999898</v>
+      </c>
+      <c r="E31">
+        <v>1520.2717999999877</v>
+      </c>
+      <c r="F31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1354,11 +1545,17 @@
       <c r="C32" s="1">
         <v>217828.47899999999</v>
       </c>
-      <c r="E32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>344.59489999999641</v>
+      </c>
+      <c r="E32">
+        <v>1410.2329999999783</v>
+      </c>
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1368,11 +1565,17 @@
       <c r="C33" s="1">
         <v>217857.43659999999</v>
       </c>
-      <c r="E33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>454.63360000000102</v>
+      </c>
+      <c r="E33">
+        <v>1439.1905999999726</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1382,11 +1585,17 @@
       <c r="C34" s="1">
         <v>217866.12390000001</v>
       </c>
-      <c r="E34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>445.94639999998617</v>
+      </c>
+      <c r="E34">
+        <v>1447.8778999999922</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1396,11 +1605,17 @@
       <c r="C35" s="1">
         <v>217906.66440000001</v>
       </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>593.62989999999991</v>
+      </c>
+      <c r="E35">
+        <v>1488.418399999995</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1410,11 +1625,17 @@
       <c r="C36" s="1">
         <v>217897.97719999999</v>
       </c>
-      <c r="E36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>602.31719999999041</v>
+      </c>
+      <c r="E36">
+        <v>1479.7311999999802</v>
+      </c>
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1424,11 +1645,17 @@
       <c r="C37" s="1">
         <v>217880.60260000001</v>
       </c>
-      <c r="E37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>599.42139999999199</v>
+      </c>
+      <c r="E37">
+        <v>1462.3565999999992</v>
+      </c>
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1438,11 +1665,17 @@
       <c r="C38" s="1">
         <v>217837.16630000001</v>
       </c>
-      <c r="E38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>457.52939999999944</v>
+      </c>
+      <c r="E38">
+        <v>1418.920299999998</v>
+      </c>
+      <c r="F38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1452,11 +1685,17 @@
       <c r="C39" s="1">
         <v>217845.8536</v>
       </c>
-      <c r="E39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>454.63360000000102</v>
+      </c>
+      <c r="E39">
+        <v>1427.6075999999885</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1466,11 +1705,17 @@
       <c r="C40" s="1">
         <v>217825.5833</v>
       </c>
-      <c r="E40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>376.44819999998435</v>
+      </c>
+      <c r="E40">
+        <v>1407.3372999999847</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1480,11 +1725,17 @@
       <c r="C41" s="1">
         <v>217756.0851</v>
       </c>
-      <c r="E41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>396.71849999998813</v>
+      </c>
+      <c r="E41">
+        <v>1337.8390999999829</v>
+      </c>
+      <c r="F41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1494,11 +1745,17 @@
       <c r="C42" s="1">
         <v>217695.27429999999</v>
       </c>
-      <c r="E42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>376.44819999998435</v>
+      </c>
+      <c r="E42">
+        <v>1277.0282999999763</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1508,11 +1765,17 @@
       <c r="C43" s="1">
         <v>217651.83790000001</v>
       </c>
-      <c r="E43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>373.55249999999069</v>
+      </c>
+      <c r="E43">
+        <v>1233.5918999999994</v>
+      </c>
+      <c r="F43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1522,11 +1785,17 @@
       <c r="C44" s="1">
         <v>217567.861</v>
       </c>
-      <c r="E44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>477.79970000000321</v>
+      </c>
+      <c r="E44">
+        <v>1149.6149999999907</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1536,11 +1805,17 @@
       <c r="C45" s="1">
         <v>217628.67189999999</v>
       </c>
-      <c r="E45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>660.23230000000331</v>
+      </c>
+      <c r="E45">
+        <v>1210.4258999999729</v>
+      </c>
+      <c r="F45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1550,14 +1825,17 @@
       <c r="C46" s="1">
         <v>217397.01139999999</v>
       </c>
-      <c r="D46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>608.10869999998249</v>
+      </c>
+      <c r="E46">
+        <v>978.76539999997476</v>
+      </c>
+      <c r="F46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1567,11 +1845,14 @@
       <c r="C47" s="1">
         <v>217475.19680000001</v>
       </c>
-      <c r="D47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>448.84209999997984</v>
+      </c>
+      <c r="E47">
+        <v>1056.9507999999914</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1581,11 +1862,14 @@
       <c r="C48" s="1">
         <v>217142.18489999999</v>
       </c>
-      <c r="D48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>222.97319999997853</v>
+      </c>
+      <c r="E48">
+        <v>723.93889999997918</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1595,11 +1879,14 @@
       <c r="C49" s="1">
         <v>217087.16560000001</v>
       </c>
-      <c r="D49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>338.80340000000433</v>
+      </c>
+      <c r="E49">
+        <v>668.91959999999381</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1609,9 +1896,24 @@
       <c r="C50" s="1">
         <v>216513.80600000001</v>
       </c>
-      <c r="D50" t="s">
-        <v>0</v>
-      </c>
+      <c r="D50">
+        <v>8.6872999999905005</v>
+      </c>
+      <c r="E50">
+        <v>95.559999999997672</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F58" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C50">

</xml_diff>

<commit_message>
The sub-polygons ready for scan
</commit_message>
<xml_diff>
--- a/test_data/antwerpen.xlsx
+++ b/test_data/antwerpen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\GitHub\Adaptive-Sonar-Route-Planning\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835142D3-EA0B-4EF6-8105-3414B6825FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD9F6F2-2CFB-4EDD-B853-1761CE0E7B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{66C3736A-0E62-4634-AFEE-C53C0DACC39D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="1">
   <si>
     <t>#</t>
   </si>
@@ -922,7 +922,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,6 +948,9 @@
         <f t="array" ref="E1:E50">C1:C50-H1</f>
         <v>98.455699999991339</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
       <c r="G1" s="1">
         <f>MIN(B1:B50)</f>
         <v>146917.83350000001</v>
@@ -973,6 +976,9 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -990,6 +996,9 @@
       <c r="E3">
         <v>486.48699999999371</v>
       </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1007,6 +1016,9 @@
       <c r="E4">
         <v>361.96949999997742</v>
       </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1024,6 +1036,9 @@
       <c r="E5">
         <v>121.62179999999353</v>
       </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1041,6 +1056,9 @@
       <c r="E6">
         <v>301.1585999999952</v>
       </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1058,6 +1076,9 @@
       <c r="E7">
         <v>561.77659999998286</v>
       </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1075,6 +1096,9 @@
       <c r="E8">
         <v>833.97769999998854</v>
       </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1851,6 +1875,9 @@
       <c r="E47">
         <v>1056.9507999999914</v>
       </c>
+      <c r="F47" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
@@ -1868,6 +1895,9 @@
       <c r="E48">
         <v>723.93889999997918</v>
       </c>
+      <c r="F48" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
@@ -1885,6 +1915,9 @@
       <c r="E49">
         <v>668.91959999999381</v>
       </c>
+      <c r="F49" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
@@ -1901,6 +1934,9 @@
       </c>
       <c r="E50">
         <v>95.559999999997672</v>
+      </c>
+      <c r="F50" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>